<commit_message>
Conditional formating and Data Cleaning
</commit_message>
<xml_diff>
--- a/Conditional Formatting Excel Tutorial File.xlsx
+++ b/Conditional Formatting Excel Tutorial File.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\OneDrive\Desktop\Ayushi\Practice\Excel\Excel-Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE12AABD-2C2A-4D60-B298-E861FD33474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58886E3-8B32-42EA-9279-C21964C3783B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Demographics" sheetId="1" r:id="rId1"/>
-    <sheet name="Sales" sheetId="4" r:id="rId2"/>
+    <sheet name="Sales" sheetId="4" r:id="rId1"/>
+    <sheet name="Demographics" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Demographics!$A$1:$K$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -333,7 +336,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -642,11 +656,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2">
+        <v>310</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>750</v>
+      </c>
+      <c r="F2">
+        <v>440</v>
+      </c>
+      <c r="G2">
+        <v>485</v>
+      </c>
+      <c r="H2">
+        <v>510</v>
+      </c>
+      <c r="I2">
+        <v>347</v>
+      </c>
+      <c r="J2">
+        <v>736</v>
+      </c>
+      <c r="K2">
+        <v>155</v>
+      </c>
+      <c r="L2">
+        <v>450</v>
+      </c>
+      <c r="M2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>71</v>
+      </c>
+      <c r="H3">
+        <v>57</v>
+      </c>
+      <c r="I3">
+        <v>61</v>
+      </c>
+      <c r="J3">
+        <v>34</v>
+      </c>
+      <c r="K3">
+        <v>41</v>
+      </c>
+      <c r="L3">
+        <v>58</v>
+      </c>
+      <c r="M3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>118</v>
+      </c>
+      <c r="D4">
+        <v>145</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>170</v>
+      </c>
+      <c r="H4">
+        <v>130</v>
+      </c>
+      <c r="I4">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>55</v>
+      </c>
+      <c r="K4">
+        <v>110</v>
+      </c>
+      <c r="L4">
+        <v>130</v>
+      </c>
+      <c r="M4">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M2">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:M3">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:M4">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +878,7 @@
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
@@ -701,264 +921,264 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H2">
-        <v>45000</v>
+        <v>36000</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="H3">
-        <v>36000</v>
+        <v>41000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1003</v>
+        <v>1009</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="H4">
-        <v>63000</v>
+        <v>42000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5">
-        <v>31</v>
-      </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>47000</v>
+        <v>45000</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>47000</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6">
-        <v>50000</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>65000</v>
+        <v>48000</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H8">
-        <v>41000</v>
+        <v>50000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1008</v>
+        <v>1003</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E9">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -967,245 +1187,118 @@
         <v>13</v>
       </c>
       <c r="H9">
-        <v>48000</v>
+        <v>63000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="H10">
-        <v>42000</v>
+        <v>65000</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D22" t="str">
-        <f t="shared" ref="D22:D23" si="0">CONCATENATE(B12," ",C12)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2">
-        <v>450</v>
-      </c>
-      <c r="C2">
-        <v>310</v>
-      </c>
-      <c r="D2">
-        <v>150</v>
-      </c>
-      <c r="E2">
-        <v>750</v>
-      </c>
-      <c r="F2">
-        <v>440</v>
-      </c>
-      <c r="G2">
-        <v>485</v>
-      </c>
-      <c r="H2">
-        <v>510</v>
-      </c>
-      <c r="I2">
-        <v>347</v>
-      </c>
-      <c r="J2">
-        <v>736</v>
-      </c>
-      <c r="K2">
-        <v>155</v>
-      </c>
-      <c r="L2">
-        <v>450</v>
-      </c>
-      <c r="M2">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-      <c r="F3">
-        <v>24</v>
-      </c>
-      <c r="G3">
-        <v>71</v>
-      </c>
-      <c r="H3">
-        <v>57</v>
-      </c>
-      <c r="I3">
-        <v>61</v>
-      </c>
-      <c r="J3">
-        <v>34</v>
-      </c>
-      <c r="K3">
-        <v>41</v>
-      </c>
-      <c r="L3">
-        <v>58</v>
-      </c>
-      <c r="M3">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
-      </c>
-      <c r="C4">
-        <v>118</v>
-      </c>
-      <c r="D4">
-        <v>145</v>
-      </c>
-      <c r="E4">
-        <v>210</v>
-      </c>
-      <c r="F4">
-        <v>45</v>
-      </c>
-      <c r="G4">
-        <v>170</v>
-      </c>
-      <c r="H4">
-        <v>130</v>
-      </c>
-      <c r="I4">
-        <v>90</v>
-      </c>
-      <c r="J4">
-        <v>55</v>
-      </c>
-      <c r="K4">
-        <v>110</v>
-      </c>
-      <c r="L4">
-        <v>130</v>
-      </c>
-      <c r="M4">
-        <v>180</v>
-      </c>
-    </row>
-  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K10">
+    <sortCondition ref="H2:H10"/>
+    <sortCondition ref="B2:B10"/>
+  </sortState>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>